<commit_message>
Update: Plumbing Client v1
</commit_message>
<xml_diff>
--- a/audio_files.xlsx
+++ b/audio_files.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Filename</t>
   </si>
@@ -30,122 +30,52 @@
     <t>Category</t>
   </si>
   <si>
-    <t xml:space="preserve">AVS International एक modern CBSE-affiliated school है, जो academic excellence के साथ-साथ बच्चों के holistic development पर भी focus करता है। हमारा campus smart classrooms, CCTV surveillance, और co-curricular activities से well-equipped है।” “हम AVS International में सिर्फ़ पढ़ाई नहीं, बल्कि overall growth पर भी बहुत ध्यान देते हैं — जैसे music, sports, और tech-based learning।
+    <t>plumbing_intro.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G’day! You’ve reached Pete's Plumbing. How can we help you today?
 </t>
   </si>
   <si>
-    <t xml:space="preserve">हमारे school में music, dance, football, basketball और skating जैसी कई activities होती हैं। Not only this, इसके अलावा भी काफ़ी नई activities हम regularly introduce करते रहते हैं.
+    <t>in_business_how_long.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We’ve been doing this for 7 years now and got loads of happy clients and repeat work. You’ll be in safe hands.
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Ofcourse! Classrooms smart boards से equipped हैं, जिससे पढ़ाई interactive और engaging होती है, बच्चों को concepts ज़्यादा अच्छे से समझ आते हैं। हर class में audio-visual teaching tools, projector-based lessons और activity-based learning modules available हैं।
+    <t>services_offered.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We handle blocked drains, leaking taps, toilet repairs, hot water issues, and a range of other plumbing issues. We also do gas fitting, pipe relining, and kitchen or bathroom plumbing. What’s the issue you’re facing right now?
 </t>
   </si>
   <si>
-    <t xml:space="preserve">बिलकुल! हमारे new students के लिए merit based scholarships available हैं, और कुछ cases में हम कुछ selected students को discounted fees भी दे सकते हैं। क्या आप चाहेंगे कि मैं अधिक जानकारी के लिए call को Admission counsellor को transfer कर दूँ?
+    <t>available_hours.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We’re available Monday through Saturday, 8am to 6pm. After-hours emergency support is also available for an extra service fee, so yeah, give us a ring anytime.
 </t>
   </si>
   <si>
-    <t xml:space="preserve">जी, AVS International में security हमारी top priority है, और हम इसे lightly नहीं लेते। हमारे स्कूल में 24 7 CCTV camera लगे हैं, और हमारी building के सभी entry और exit points पर security guards, active रहते हैं। इसके अलावा, हमारे कुछ teachers and staff हमेशा corridors में regularly घूमते रहते हैं ताकि internally bhi कोई mischief न हो।
+    <t>pricing.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our pricing usually starts at $98 for standard service calls. We’ll provide a full quote after understanding the job better.
 </t>
   </si>
   <si>
-    <t xml:space="preserve">सुनकर बहुत अच्छा लगा। Actually, हमने बहुत सारे events plan किए हैं, जैसे dance, music, bike show भी होगा, और students ने एक patriotic play के लिए भी खूब मेहनत की है। So yeah [chuckle], इस साल के लिए बहुत कुछ plan किया गया है।
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fantastic! Actually, मैंने आपको यह बताने के लिए call किया था कि AVS International, 18 september को अपना annual function host कर रहा है, और हम चाहते हैं कि आप इस function का हिस्सा बनें। क्या आप इसमें interested हैं ?
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">नमस्ते मै निशा बोल रही हूँ from AVS International School. क्या आपके पास जल्दी से बात करने के लिए 2 मिनट हैं?
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admission Form जमा करने की last date 15 March है। Around 25th March, onboarding and assessment procedure शुरू हो जाएगी.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ji हाँ, हमारा स्कूल CBSE based है।
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">School timings are, Monday से Friday सुबह आठ बजे से दोपहर दो बजे तक है।
-</t>
-  </si>
-  <si>
-    <t>Ofcourse! Please बताएं student कहां से bus में चढ़ना चाहता है?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">बिल्कुल! Fees के बारे में, क्या मैं आपके बच्चे के admission की class के बारे में जान सक्ती हूँ? यह उसी पर depend करता है।
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">जी बिल्कुल! आप स्कूल से admission form प्राप्त कर सकते हैं या हमारी website से download कर सकते हैं। form को required documents के साथ जमा करें। आपको birth certificate और passport size photo की आवश्यकता होगी। क्योंकि दूसरे स्कूल से student का ट्रांसफर हो रहा है, तो आपका पिछले स्कूल से एक transfer certificate भी लेकर हमें फॉर्म के साथ जमा करना होगा. Form submit करने के बाद, हम आपको और आपके बच्चे को onboarding interview के लिए invite करेंगे, साथ ही आपके बच्चे को एक pre assessment exam भी देनी पड़ सकती है, क्योंकि हमारी admission procedures kaafi strict है।
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">जी बिल्कुल! आप स्कूल से admission form प्राप्त कर सकते हैं या हमारी website से download कर सकते हैं। form को required documents के साथ जमा करें। आपको birth certificate और passport size photo की आवश्यकता होगी। Form submit करने के बाद, हम आपको और आपके बच्चे को onboarding interview के लिए invite करेंगे, साथ ही आपके बच्चे को एक pre assessment exam भी देनी पड़ सकती है, क्योंकि हमारी admission procedures kaafi strict है।
-</t>
-  </si>
-  <si>
-    <t>admission_process_firsttime.mp3</t>
-  </si>
-  <si>
-    <t>admission_process_transfer.mp3</t>
-  </si>
-  <si>
-    <t>fees_ask_class.mp3</t>
-  </si>
-  <si>
-    <t>bus_ask_location.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">जी bus की fees लगभग 500 से 800 रुपये होती है, लेकिन आप इसे और confirm करने के लिए एक बार school आके बात कर लीजिये।
-</t>
-  </si>
-  <si>
-    <t>school_timings.mp3</t>
-  </si>
-  <si>
-    <t>bus_fees.mp3</t>
-  </si>
-  <si>
-    <t>cbse_based.mp3</t>
-  </si>
-  <si>
-    <t>admission_last_date.mp3</t>
-  </si>
-  <si>
-    <t>nisha_introduction_outbound.mp3</t>
-  </si>
-  <si>
-    <t>annual_function_invite.mp3</t>
-  </si>
-  <si>
-    <t>annual_function_events.mp3</t>
-  </si>
-  <si>
-    <t>security.mp3</t>
-  </si>
-  <si>
-    <t>scholarships_n_discounts.mp3</t>
-  </si>
-  <si>
-    <t>smart_classes.mp3</t>
-  </si>
-  <si>
-    <t>extra_activities.mp3</t>
-  </si>
-  <si>
-    <t>school_intro.mp3</t>
+    <t>ask_time_day.mp3</t>
+  </si>
+  <si>
+    <t>We’ve got a few open slots this week. What time and day works for you?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,11 +106,6 @@
       <name val="Inter"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Roboto"/>
     </font>
@@ -194,6 +119,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -380,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -416,29 +354,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -450,6 +382,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -746,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -758,177 +697,137 @@
     <col min="5" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:4" s="25" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="24" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="90" thickBot="1">
-      <c r="A2" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="15" t="s">
+    <row r="2" spans="1:4" ht="39" thickBot="1">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16"/>
+      <c r="B2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="64.5" thickBot="1">
-      <c r="A3" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19"/>
-    </row>
-    <row r="4" spans="1:4" ht="77.25" thickBot="1">
-      <c r="A4" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="15" t="s">
+      <c r="A3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="21"/>
-    </row>
-    <row r="5" spans="1:4" ht="77.25" thickBot="1">
-      <c r="A5" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="15" t="s">
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="21"/>
-    </row>
-    <row r="6" spans="1:4" ht="90" thickBot="1">
+      <c r="C3" s="16"/>
+      <c r="D3" s="17"/>
+    </row>
+    <row r="4" spans="1:4" ht="64.5" thickBot="1">
+      <c r="A4" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="1:4" ht="64.5" thickBot="1">
+      <c r="A5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="19"/>
+    </row>
+    <row r="6" spans="1:4" ht="51.75" thickBot="1">
       <c r="A6" s="7" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:4" ht="64.5" thickBot="1">
+    <row r="7" spans="1:4" ht="13.5" thickBot="1">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" ht="64.5" thickBot="1">
-      <c r="A8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>10</v>
-      </c>
+    <row r="8" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="51.75" thickBot="1">
-      <c r="A9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>11</v>
-      </c>
+    <row r="9" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" ht="51.75" thickBot="1">
-      <c r="A10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
+    <row r="10" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" ht="39" thickBot="1">
-      <c r="A11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>13</v>
-      </c>
+    <row r="11" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" ht="51.75" thickBot="1">
-      <c r="A12" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="24"/>
-    </row>
-    <row r="13" spans="1:4" ht="39" thickBot="1">
-      <c r="A13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>14</v>
-      </c>
+    <row r="12" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="22"/>
+    </row>
+    <row r="13" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="2"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" ht="51.75" thickBot="1">
-      <c r="A15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>16</v>
-      </c>
+    <row r="15" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:4" ht="128.25" thickBot="1">
-      <c r="A16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>17</v>
-      </c>
+    <row r="16" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" ht="102.75" thickBot="1">
-      <c r="A17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>18</v>
-      </c>
+    <row r="17" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="5"/>
     </row>

</xml_diff>